<commit_message>
Add goal deduction in confirmDraftOrder
</commit_message>
<xml_diff>
--- a/data/distributor_location.xlsx
+++ b/data/distributor_location.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\tickin-backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85D512A-548F-4C71-8FDD-7A5C46575BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3E2CEE-37D6-4697-A44E-ADB4066CD176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -795,13 +795,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="A1:E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
     <col min="3" max="3" width="35.5703125" customWidth="1"/>
     <col min="4" max="4" width="29.85546875" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" customWidth="1"/>

</xml_diff>